<commit_message>
update automation script and browserstack automation script video url
</commit_message>
<xml_diff>
--- a/DataSheet/IshinePortal.xlsx
+++ b/DataSheet/IshinePortal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BiswajitFramework\DataSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BiswajitFramework3\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E24E32-74F6-4733-8603-1150698BC279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D6B844-14C8-44D1-BCC8-76AC4A6E3CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B5C4A126-B641-4661-957C-F82AF751E901}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="226">
   <si>
     <t>Si No</t>
   </si>
@@ -699,6 +699,12 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>(//a[@id='user-dropdown'])[1]</t>
+  </si>
+  <si>
+    <t>(//a[@class = 'dropdown-item'])[2]</t>
   </si>
 </sst>
 </file>
@@ -2028,10 +2034,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE73440-ADC0-400F-94D2-AEBDBE56EBE3}">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2941,7 +2947,7 @@
         <v>213</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>223</v>
       </c>
       <c r="E30" t="s">
         <v>155</v>
@@ -2973,7 +2979,7 @@
         <v>213</v>
       </c>
       <c r="D31" t="s">
-        <v>223</v>
+        <v>12</v>
       </c>
       <c r="H31" t="s">
         <v>87</v>
@@ -3371,8 +3377,8 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>40</v>
+      <c r="A45" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="B45" t="s">
         <v>78</v>
@@ -3383,8 +3389,14 @@
       <c r="D45" t="s">
         <v>12</v>
       </c>
+      <c r="E45" t="s">
+        <v>70</v>
+      </c>
+      <c r="F45" t="s">
+        <v>224</v>
+      </c>
       <c r="H45" t="s">
-        <v>152</v>
+        <v>72</v>
       </c>
       <c r="J45" t="s">
         <v>171</v>
@@ -3393,6 +3405,64 @@
         <v>220</v>
       </c>
       <c r="L45" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" t="s">
+        <v>214</v>
+      </c>
+      <c r="D46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" t="s">
+        <v>70</v>
+      </c>
+      <c r="F46" t="s">
+        <v>225</v>
+      </c>
+      <c r="H46" t="s">
+        <v>72</v>
+      </c>
+      <c r="J46" t="s">
+        <v>171</v>
+      </c>
+      <c r="K46" t="s">
+        <v>220</v>
+      </c>
+      <c r="L46" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>40</v>
+      </c>
+      <c r="B47" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" t="s">
+        <v>214</v>
+      </c>
+      <c r="D47" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" t="s">
+        <v>152</v>
+      </c>
+      <c r="J47" t="s">
+        <v>171</v>
+      </c>
+      <c r="K47" t="s">
+        <v>220</v>
+      </c>
+      <c r="L47" t="s">
         <v>210</v>
       </c>
     </row>

</xml_diff>